<commit_message>
complete calculate.c not tested good job
</commit_message>
<xml_diff>
--- a/附加文件/word的label的对应表.xlsx
+++ b/附加文件/word的label的对应表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Want to change isMatrix
</commit_message>
<xml_diff>
--- a/附加文件/word的label的对应表.xlsx
+++ b/附加文件/word的label的对应表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="103">
   <si>
     <t>:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -417,6 +417,14 @@
   </si>
   <si>
     <t>空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>solve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -775,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1697,12 +1705,23 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B49">
         <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>